<commit_message>
Adding instructions document and fixes
</commit_message>
<xml_diff>
--- a/src/main/java/data/waesdata.xlsx
+++ b/src/main/java/data/waesdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Varios\Entrevistas\waes-test\src\main\java\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304F6DE3-E094-4EF5-9B69-B822D709860E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C705CFF2-A41A-4215-97DF-7F9963B5E1E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{30F17799-0A18-4BA2-A76D-8633784C3C58}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="171">
+  <dxfs count="165">
     <dxf>
       <font>
         <b/>
@@ -973,48 +976,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2120,7 +2081,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2294,7 +2255,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2774,7 +2735,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2806,7 +2767,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2844,299 +2805,299 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B10:I16">
-    <cfRule type="expression" dxfId="170" priority="84">
+    <cfRule type="expression" dxfId="164" priority="84">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="85">
+    <cfRule type="expression" dxfId="163" priority="85">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="86">
+    <cfRule type="expression" dxfId="162" priority="86">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:I16">
-    <cfRule type="containsText" dxfId="167" priority="79" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="161" priority="79" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="80" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="160" priority="80" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="81" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="159" priority="81" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17 B18:C18 E17:I17 B19:D19 F18:I18 B20:E20 G19:I19 B21:F21 H20:I20 B22:G22 I21">
-    <cfRule type="containsText" dxfId="164" priority="73" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="158" priority="73" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="74" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="157" priority="74" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="75" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="156" priority="75" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="161" priority="70">
+    <cfRule type="expression" dxfId="155" priority="70">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="71">
+    <cfRule type="expression" dxfId="154" priority="71">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="72">
+    <cfRule type="expression" dxfId="153" priority="72">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="containsText" dxfId="158" priority="67" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="152" priority="67" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="68" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="151" priority="68" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",C17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="69" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="150" priority="69" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="155" priority="64">
+    <cfRule type="expression" dxfId="149" priority="64">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="65">
+    <cfRule type="expression" dxfId="148" priority="65">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="66">
+    <cfRule type="expression" dxfId="147" priority="66">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="152" priority="61" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="146" priority="61" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="62" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="145" priority="62" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",D17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="63" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="144" priority="63" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",D17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="149" priority="58">
+    <cfRule type="expression" dxfId="143" priority="58">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="59">
+    <cfRule type="expression" dxfId="142" priority="59">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="60">
+    <cfRule type="expression" dxfId="141" priority="60">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="146" priority="55" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="140" priority="55" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="56" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="139" priority="56" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",D18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="57" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="138" priority="57" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",D18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="143" priority="52">
+    <cfRule type="expression" dxfId="137" priority="52">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="53">
+    <cfRule type="expression" dxfId="136" priority="53">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="54">
+    <cfRule type="expression" dxfId="135" priority="54">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="containsText" dxfId="140" priority="49" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="134" priority="49" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="50" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="133" priority="50" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",E18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="51" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="132" priority="51" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",E18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="137" priority="46">
+    <cfRule type="expression" dxfId="131" priority="46">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="47">
+    <cfRule type="expression" dxfId="130" priority="47">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="48">
+    <cfRule type="expression" dxfId="129" priority="48">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="containsText" dxfId="134" priority="43" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="128" priority="43" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",E19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="44" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="127" priority="44" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",E19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="45" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="126" priority="45" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",E19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="131" priority="40">
+    <cfRule type="expression" dxfId="125" priority="40">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="41">
+    <cfRule type="expression" dxfId="124" priority="41">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="42">
+    <cfRule type="expression" dxfId="123" priority="42">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="128" priority="37" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="122" priority="37" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="38" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="121" priority="38" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="39" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="120" priority="39" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",F19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="125" priority="34">
+    <cfRule type="expression" dxfId="119" priority="34">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="35">
+    <cfRule type="expression" dxfId="118" priority="35">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="36">
+    <cfRule type="expression" dxfId="117" priority="36">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="containsText" dxfId="122" priority="31" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="116" priority="31" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",F20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="32" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="115" priority="32" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",F20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="33" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="114" priority="33" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",F20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="expression" dxfId="119" priority="28">
+    <cfRule type="expression" dxfId="113" priority="28">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="29">
+    <cfRule type="expression" dxfId="112" priority="29">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="30">
+    <cfRule type="expression" dxfId="111" priority="30">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="containsText" dxfId="116" priority="25" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="110" priority="25" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="26" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="109" priority="26" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="27" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="108" priority="27" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="expression" dxfId="113" priority="22">
+    <cfRule type="expression" dxfId="107" priority="22">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="23">
+    <cfRule type="expression" dxfId="106" priority="23">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="24">
+    <cfRule type="expression" dxfId="105" priority="24">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21">
-    <cfRule type="containsText" dxfId="110" priority="19" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="104" priority="19" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",G21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="20" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="103" priority="20" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",G21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="21" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="102" priority="21" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="expression" dxfId="107" priority="16">
+    <cfRule type="expression" dxfId="101" priority="16">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="17">
+    <cfRule type="expression" dxfId="100" priority="17">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="18">
+    <cfRule type="expression" dxfId="99" priority="18">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="104" priority="13" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="98" priority="13" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",H21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="14" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="97" priority="14" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",H21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="15" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="96" priority="15" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",H21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="101" priority="10">
+    <cfRule type="expression" dxfId="95" priority="10">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="11">
+    <cfRule type="expression" dxfId="94" priority="11">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="12">
+    <cfRule type="expression" dxfId="93" priority="12">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="containsText" dxfId="98" priority="7" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="92" priority="7" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",H22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="91" priority="8" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",H22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="90" priority="9" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",H22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="expression" dxfId="95" priority="4">
+    <cfRule type="expression" dxfId="89" priority="4">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="5">
+    <cfRule type="expression" dxfId="88" priority="5">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="6">
+    <cfRule type="expression" dxfId="87" priority="6">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22">
-    <cfRule type="containsText" dxfId="92" priority="1" operator="containsText" text="EMPTY">
+    <cfRule type="containsText" dxfId="86" priority="1" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="2" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="85" priority="2" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",I22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="84" priority="3" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",I22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3159,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{747DD830-0D78-4AB6-92E0-8F370C84190E}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3208,13 +3169,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -3240,13 +3201,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>19</v>
@@ -3272,7 +3233,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>20</v>
@@ -3284,7 +3245,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>20</v>
@@ -3304,7 +3265,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>20</v>
@@ -3316,10 +3277,10 @@
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>20</v>
@@ -3336,7 +3297,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>20</v>
@@ -3351,10 +3312,10 @@
         <v>20</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>20</v>
@@ -3368,7 +3329,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>20</v>
@@ -3386,10 +3347,10 @@
         <v>20</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>19</v>
@@ -3400,7 +3361,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
@@ -3421,7 +3382,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>19</v>
@@ -3432,13 +3393,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>19</v>
@@ -3464,13 +3425,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
@@ -3496,7 +3457,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>20</v>
@@ -3508,7 +3469,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>20</v>
@@ -3523,12 +3484,12 @@
         <v>19</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>20</v>
@@ -3540,10 +3501,10 @@
         <v>19</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>20</v>
@@ -3555,12 +3516,12 @@
         <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
@@ -3575,10 +3536,10 @@
         <v>20</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>20</v>
@@ -3592,7 +3553,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>20</v>
@@ -3610,10 +3571,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>19</v>
@@ -3624,7 +3585,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>20</v>
@@ -3645,7 +3606,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>19</v>
@@ -3656,13 +3617,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>19</v>
@@ -3680,7 +3641,7 @@
         <v>20</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>37</v>
@@ -3688,19 +3649,19 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>20</v>
@@ -3715,12 +3676,12 @@
         <v>20</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>20</v>
@@ -3729,13 +3690,13 @@
         <v>20</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>20</v>
@@ -3752,7 +3713,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>20</v>
@@ -3764,13 +3725,13 @@
         <v>20</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>20</v>
@@ -3779,12 +3740,12 @@
         <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>20</v>
@@ -3799,24 +3760,24 @@
         <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>20</v>
@@ -3834,107 +3795,53 @@
         <v>20</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C10:I16">
-    <cfRule type="expression" dxfId="89" priority="88">
+  <conditionalFormatting sqref="C9:I15 D2:D15 I2:I15">
+    <cfRule type="expression" dxfId="83" priority="88">
       <formula>"MISSING"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="89">
+    <cfRule type="expression" dxfId="82" priority="89">
       <formula>"EMPTY"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="90">
+    <cfRule type="expression" dxfId="81" priority="90">
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I3 C4:I16">
-    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="EMPTY">
+  <conditionalFormatting sqref="C3:I15 B2:I2">
+    <cfRule type="containsText" dxfId="80" priority="85" operator="containsText" text="EMPTY">
       <formula>NOT(ISERROR(SEARCH("EMPTY",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="MISSING">
+    <cfRule type="containsText" dxfId="79" priority="86" operator="containsText" text="MISSING">
       <formula>NOT(ISERROR(SEARCH("MISSING",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="FILLED">
+    <cfRule type="containsText" dxfId="78" priority="87" operator="containsText" text="FILLED">
       <formula>NOT(ISERROR(SEARCH("FILLED",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D16">
-    <cfRule type="expression" dxfId="83" priority="82">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="83">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="84">
-      <formula>"""FILLED"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
-    <cfRule type="expression" dxfId="80" priority="79">
-      <formula>"MISSING"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="79" priority="80">
-      <formula>"EMPTY"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="81">
-      <formula>"""FILLED"""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C18 E17:I17 C19:D19 F18:I18 C20:E20 G19:I19 C21:F21 H20:I20 C22:G22 I21">
+  <conditionalFormatting sqref="C17 E16:I16 C18:D18 F17:I17 C19:E19 G18:I18 C20:F20 H19:I19 C21:G21 I20">
     <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+      <formula>NOT(ISERROR(SEARCH("FILLED",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
     <cfRule type="expression" dxfId="74" priority="73">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -3945,18 +3852,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="C16">
     <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",C17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",C16)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",C17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+      <formula>NOT(ISERROR(SEARCH("FILLED",C16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
     <cfRule type="expression" dxfId="68" priority="67">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -3967,18 +3874,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",D16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",D16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",D17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",D17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
     <cfRule type="expression" dxfId="62" priority="61">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -3989,18 +3896,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
+  <conditionalFormatting sqref="D17">
     <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",D18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",D17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",D18)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",D17)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",D18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
+      <formula>NOT(ISERROR(SEARCH("FILLED",D17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
     <cfRule type="expression" dxfId="56" priority="55">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4011,18 +3918,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",E17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",E17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",E18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",E18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
     <cfRule type="expression" dxfId="50" priority="49">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4033,18 +3940,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
+  <conditionalFormatting sqref="E18">
     <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",E19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",E18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",E19)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",E18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",E19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
+      <formula>NOT(ISERROR(SEARCH("FILLED",E18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
     <cfRule type="expression" dxfId="44" priority="43">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4055,18 +3962,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",F18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",F18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",F18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",F19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",F19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",F19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
     <cfRule type="expression" dxfId="38" priority="37">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4077,18 +3984,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
+  <conditionalFormatting sqref="F19">
     <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",F20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",F19)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",F20)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",F19)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",F20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+      <formula>NOT(ISERROR(SEARCH("FILLED",F19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
     <cfRule type="expression" dxfId="32" priority="31">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4099,18 +4006,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G19">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",G19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",G19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",G19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",G20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",G20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",G20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
     <cfRule type="expression" dxfId="26" priority="25">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4121,18 +4028,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
+  <conditionalFormatting sqref="G20">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",G21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",G20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",G21)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",G20)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",G21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
+      <formula>NOT(ISERROR(SEARCH("FILLED",G20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4143,18 +4050,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="EMPTY">
+      <formula>NOT(ISERROR(SEARCH("EMPTY",H20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="MISSING">
+      <formula>NOT(ISERROR(SEARCH("MISSING",H20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="FILLED">
+      <formula>NOT(ISERROR(SEARCH("FILLED",H20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",H21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",H21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",H21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
     <cfRule type="expression" dxfId="14" priority="13">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4165,18 +4072,18 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H21">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",H22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",H21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",H22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",H21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",H22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+      <formula>NOT(ISERROR(SEARCH("FILLED",H21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I21">
     <cfRule type="expression" dxfId="8" priority="7">
       <formula>"MISSING"</formula>
     </cfRule>
@@ -4187,26 +4094,26 @@
       <formula>"""FILLED"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I22">
+  <conditionalFormatting sqref="I21">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",I22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",I21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",I22)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",I21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",I22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B22">
+      <formula>NOT(ISERROR(SEARCH("FILLED",I21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B21">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="EMPTY">
-      <formula>NOT(ISERROR(SEARCH("EMPTY",B4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("EMPTY",B3)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="MISSING">
-      <formula>NOT(ISERROR(SEARCH("MISSING",B4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("MISSING",B3)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FILLED">
-      <formula>NOT(ISERROR(SEARCH("FILLED",B4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FILLED",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4217,7 +4124,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:I22</xm:sqref>
+          <xm:sqref>B2:I21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>